<commit_message>
backup before dimension reduction
</commit_message>
<xml_diff>
--- a/gams/matchingRAData_priceNeg_Q1.xlsx
+++ b/gams/matchingRAData_priceNeg_Q1.xlsx
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>q1</t>
+          <t>q0</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -527,7 +527,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>q2</t>
+          <t>q1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -559,7 +559,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>q3</t>
+          <t>q2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -591,7 +591,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>q4</t>
+          <t>q3</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -621,7 +621,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>q5</t>
+          <t>q4</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -659,7 +659,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>q6</t>
+          <t>q5</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -697,7 +697,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>q7</t>
+          <t>q6</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -733,7 +733,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>q8</t>
+          <t>q7</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -765,7 +765,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>q9</t>
+          <t>q8</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -801,7 +801,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>q10</t>
+          <t>q9</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -837,7 +837,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>q11</t>
+          <t>q10</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -875,7 +875,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>q12</t>
+          <t>q11</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -911,7 +911,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>q13</t>
+          <t>q12</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -951,7 +951,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>q14</t>
+          <t>q13</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -991,7 +991,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>q15</t>
+          <t>q14</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1031,7 +1031,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>q16</t>
+          <t>q15</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1071,7 +1071,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>q17</t>
+          <t>q16</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1107,7 +1107,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>q18</t>
+          <t>q17</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1143,7 +1143,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>q19</t>
+          <t>q18</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -1175,7 +1175,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>q20</t>
+          <t>q19</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1213,7 +1213,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>q21</t>
+          <t>q20</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1251,7 +1251,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>q22</t>
+          <t>q21</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1285,7 +1285,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>q23</t>
+          <t>q22</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1321,7 +1321,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>q24</t>
+          <t>q23</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1359,7 +1359,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>q25</t>
+          <t>q24</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1387,7 +1387,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>q26</t>
+          <t>q25</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1419,7 +1419,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>q27</t>
+          <t>q26</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1449,7 +1449,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>q28</t>
+          <t>q27</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1485,7 +1485,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>q29</t>
+          <t>q28</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1517,7 +1517,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>q30</t>
+          <t>q29</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1541,7 +1541,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>q31</t>
+          <t>q30</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1565,7 +1565,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>q32</t>
+          <t>q31</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1599,7 +1599,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>q33</t>
+          <t>q32</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1633,7 +1633,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>q34</t>
+          <t>q33</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1663,7 +1663,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>q35</t>
+          <t>q34</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1685,7 +1685,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>q36</t>
+          <t>q35</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1709,7 +1709,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>q37</t>
+          <t>q36</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1733,7 +1733,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>q38</t>
+          <t>q37</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1757,7 +1757,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>q39</t>
+          <t>q38</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1781,7 +1781,7 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>q40</t>
+          <t>q39</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1805,7 +1805,7 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>q41</t>
+          <t>q40</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1831,7 +1831,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>q42</t>
+          <t>q41</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1855,7 +1855,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>q43</t>
+          <t>q42</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1879,7 +1879,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>q44</t>
+          <t>q43</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1903,7 +1903,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>q45</t>
+          <t>q44</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1921,7 +1921,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>q46</t>
+          <t>q45</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1941,7 +1941,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>q47</t>
+          <t>q46</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1967,7 +1967,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>q48</t>
+          <t>q47</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1993,7 +1993,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>q49</t>
+          <t>q48</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -2017,7 +2017,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>q50</t>
+          <t>q49</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -2039,7 +2039,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>q51</t>
+          <t>q50</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -2071,7 +2071,7 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>q52</t>
+          <t>q51</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -2101,7 +2101,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>q53</t>
+          <t>q52</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -2123,7 +2123,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>q54</t>
+          <t>q53</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -2149,7 +2149,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>q55</t>
+          <t>q54</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -2185,7 +2185,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>q56</t>
+          <t>q55</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -2217,7 +2217,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>q57</t>
+          <t>q56</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -2241,7 +2241,7 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>q58</t>
+          <t>q57</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -2265,7 +2265,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>q59</t>
+          <t>q58</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -2291,7 +2291,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>q60</t>
+          <t>q59</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -2319,7 +2319,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>q61</t>
+          <t>q60</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -2345,7 +2345,7 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>q62</t>
+          <t>q61</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -2369,7 +2369,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>q63</t>
+          <t>q62</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -2399,7 +2399,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>q64</t>
+          <t>q63</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -2429,7 +2429,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>q65</t>
+          <t>q64</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -2455,7 +2455,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>q66</t>
+          <t>q65</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -2483,7 +2483,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>q67</t>
+          <t>q66</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -2513,7 +2513,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>q68</t>
+          <t>q67</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -2541,7 +2541,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>q69</t>
+          <t>q68</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -2575,7 +2575,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>q70</t>
+          <t>q69</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -2605,7 +2605,7 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>q71</t>
+          <t>q70</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -2635,7 +2635,7 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>q72</t>
+          <t>q71</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -2671,7 +2671,7 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>q73</t>
+          <t>q72</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -2705,7 +2705,7 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>q74</t>
+          <t>q73</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -2741,7 +2741,7 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>q75</t>
+          <t>q74</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -2777,7 +2777,7 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>q76</t>
+          <t>q75</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -2807,7 +2807,7 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>q77</t>
+          <t>q76</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -2841,7 +2841,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>q78</t>
+          <t>q77</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -2877,7 +2877,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>q79</t>
+          <t>q78</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -2915,7 +2915,7 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>q80</t>
+          <t>q79</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -2947,7 +2947,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>q81</t>
+          <t>q80</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -2979,7 +2979,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>q82</t>
+          <t>q81</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -3017,7 +3017,7 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>q83</t>
+          <t>q82</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -3053,7 +3053,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>q84</t>
+          <t>q83</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -3087,7 +3087,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>q85</t>
+          <t>q84</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -3119,7 +3119,7 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>q86</t>
+          <t>q85</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -3155,7 +3155,7 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>q87</t>
+          <t>q86</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -3193,7 +3193,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>q88</t>
+          <t>q87</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -3229,7 +3229,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>q89</t>
+          <t>q88</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -3263,7 +3263,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>q90</t>
+          <t>q89</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -3297,7 +3297,7 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>q91</t>
+          <t>q90</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -3333,7 +3333,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>q92</t>
+          <t>q91</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -3365,7 +3365,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>q93</t>
+          <t>q92</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -3399,7 +3399,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>q94</t>
+          <t>q93</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -3435,7 +3435,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>q95</t>
+          <t>q94</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -3471,7 +3471,7 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>q96</t>
+          <t>q95</t>
         </is>
       </c>
       <c r="B97" t="n">

</xml_diff>